<commit_message>
docs: fourth sprint planning
</commit_message>
<xml_diff>
--- a/docs/process/product-backlog.xlsx
+++ b/docs/process/product-backlog.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Priority</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>L'utente, oltre alla scacchiera, deve poter visualizzare tutte le restanti informazioni relative allo stato corrente della partita</t>
+  </si>
+  <si>
+    <t>Quality Assurance</t>
   </si>
 </sst>
 </file>
@@ -396,7 +399,7 @@
     <row r="4">
       <c r="A4" s="5"/>
       <c r="B4" s="6">
-        <f t="shared" ref="B4:B9" si="1">B3 + 1</f>
+        <f t="shared" ref="B4:B10" si="1">B3 + 1</f>
         <v>2</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -478,9 +481,16 @@
     </row>
     <row r="10">
       <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="10"/>
+      <c r="B10" s="6">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="6">
+        <v>6.0</v>
+      </c>
       <c r="E10" s="8"/>
     </row>
     <row r="11">

</xml_diff>